<commit_message>
R testing updates mostly
</commit_message>
<xml_diff>
--- a/sample_info_sorting.xlsx
+++ b/sample_info_sorting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="100" windowWidth="25600" windowHeight="19660" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="4160" yWindow="120" windowWidth="25600" windowHeight="19660" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1653,8 +1653,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1847,7 +1848,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="507">
+  <cellStyleXfs count="511">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2355,8 +2356,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2429,8 +2434,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="507">
+  <cellStyles count="511">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2684,6 +2690,8 @@
     <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2937,6 +2945,8 @@
     <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5656,13 +5666,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="I133" workbookViewId="0">
+      <selection activeCell="N139" sqref="N139:N162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.5" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
@@ -5670,7 +5680,7 @@
     <col min="9" max="9" width="28.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28.5" customWidth="1"/>
     <col min="16" max="16" width="21.6640625" customWidth="1"/>
   </cols>
@@ -8231,7 +8241,7 @@
     </row>
     <row r="70" spans="1:16">
       <c r="A70" s="26"/>
-      <c r="B70">
+      <c r="B70" s="28">
         <v>6666666.1646299995</v>
       </c>
       <c r="C70" t="s">
@@ -8271,7 +8281,7 @@
     </row>
     <row r="71" spans="1:16">
       <c r="A71" s="26"/>
-      <c r="B71">
+      <c r="B71" s="28">
         <v>6666666.1646389998</v>
       </c>
       <c r="C71" t="s">
@@ -8311,7 +8321,7 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" s="26"/>
-      <c r="B72">
+      <c r="B72" s="28">
         <v>6666666.1646400001</v>
       </c>
       <c r="C72" t="s">
@@ -8351,7 +8361,7 @@
     </row>
     <row r="73" spans="1:16">
       <c r="A73" s="26"/>
-      <c r="B73">
+      <c r="B73" s="28">
         <v>6666666.1646410003</v>
       </c>
       <c r="C73" t="s">
@@ -8391,7 +8401,7 @@
     </row>
     <row r="74" spans="1:16">
       <c r="A74" s="26"/>
-      <c r="B74">
+      <c r="B74" s="28">
         <v>6666666.1646419996</v>
       </c>
       <c r="C74" t="s">
@@ -8431,7 +8441,7 @@
     </row>
     <row r="75" spans="1:16">
       <c r="A75" s="26"/>
-      <c r="B75">
+      <c r="B75" s="28">
         <v>6666666.1646429999</v>
       </c>
       <c r="C75" t="s">
@@ -8471,7 +8481,7 @@
     </row>
     <row r="76" spans="1:16">
       <c r="A76" s="26"/>
-      <c r="B76" s="26">
+      <c r="B76" s="28">
         <v>6666666.1646459997</v>
       </c>
       <c r="C76" s="26" t="s">
@@ -8511,7 +8521,7 @@
     </row>
     <row r="77" spans="1:16">
       <c r="A77" s="26"/>
-      <c r="B77" s="26">
+      <c r="B77" s="28">
         <v>6666666.1646469999</v>
       </c>
       <c r="C77" s="26" t="s">
@@ -8551,7 +8561,7 @@
     </row>
     <row r="78" spans="1:16">
       <c r="A78" s="26"/>
-      <c r="B78" s="26">
+      <c r="B78" s="28">
         <v>6666666.1646480002</v>
       </c>
       <c r="C78" s="26" t="s">
@@ -8591,7 +8601,7 @@
     </row>
     <row r="79" spans="1:16">
       <c r="A79" s="26"/>
-      <c r="B79" s="26">
+      <c r="B79" s="28">
         <v>6666666.1646499997</v>
       </c>
       <c r="C79" s="26" t="s">
@@ -8631,7 +8641,7 @@
     </row>
     <row r="80" spans="1:16">
       <c r="A80" s="26"/>
-      <c r="B80" s="26">
+      <c r="B80" s="28">
         <v>6666666.1646509999</v>
       </c>
       <c r="C80" s="26" t="s">
@@ -8671,7 +8681,7 @@
     </row>
     <row r="81" spans="1:16">
       <c r="A81" s="26"/>
-      <c r="B81" s="26">
+      <c r="B81" s="28">
         <v>6666666.1646560002</v>
       </c>
       <c r="C81" s="26" t="s">
@@ -10091,7 +10101,7 @@
       <c r="K139" s="26"/>
       <c r="L139" s="26"/>
       <c r="M139" s="26"/>
-      <c r="N139">
+      <c r="N139" s="28">
         <v>6666666.1644329997</v>
       </c>
       <c r="O139" t="s">
@@ -10115,7 +10125,7 @@
       <c r="K140" s="26"/>
       <c r="L140" s="26"/>
       <c r="M140" s="26"/>
-      <c r="N140">
+      <c r="N140" s="28">
         <v>6666666.1644339999</v>
       </c>
       <c r="O140" t="s">
@@ -10139,7 +10149,7 @@
       <c r="K141" s="26"/>
       <c r="L141" s="26"/>
       <c r="M141" s="26"/>
-      <c r="N141">
+      <c r="N141" s="28">
         <v>6666666.1644350002</v>
       </c>
       <c r="O141" t="s">
@@ -10163,7 +10173,7 @@
       <c r="K142" s="26"/>
       <c r="L142" s="26"/>
       <c r="M142" s="26"/>
-      <c r="N142">
+      <c r="N142" s="28">
         <v>6666666.1644360004</v>
       </c>
       <c r="O142" t="s">
@@ -10187,7 +10197,7 @@
       <c r="K143" s="26"/>
       <c r="L143" s="26"/>
       <c r="M143" s="26"/>
-      <c r="N143">
+      <c r="N143" s="28">
         <v>6666666.1644369997</v>
       </c>
       <c r="O143" t="s">
@@ -10211,7 +10221,7 @@
       <c r="K144" s="26"/>
       <c r="L144" s="26"/>
       <c r="M144" s="26"/>
-      <c r="N144" s="26">
+      <c r="N144" s="28">
         <v>6666666.1644379999</v>
       </c>
       <c r="O144" s="26" t="s">
@@ -10235,7 +10245,7 @@
       <c r="K145" s="26"/>
       <c r="L145" s="26"/>
       <c r="M145" s="26"/>
-      <c r="N145" s="26">
+      <c r="N145" s="28">
         <v>6666666.1644390002</v>
       </c>
       <c r="O145" s="26" t="s">
@@ -10259,7 +10269,7 @@
       <c r="K146" s="26"/>
       <c r="L146" s="26"/>
       <c r="M146" s="26"/>
-      <c r="N146" s="26">
+      <c r="N146" s="28">
         <v>6666666.1644400004</v>
       </c>
       <c r="O146" s="26" t="s">
@@ -10283,7 +10293,7 @@
       <c r="K147" s="26"/>
       <c r="L147" s="26"/>
       <c r="M147" s="26"/>
-      <c r="N147" s="26">
+      <c r="N147" s="28">
         <v>6666666.1644409997</v>
       </c>
       <c r="O147" s="26" t="s">
@@ -10307,7 +10317,7 @@
       <c r="K148" s="26"/>
       <c r="L148" s="26"/>
       <c r="M148" s="26"/>
-      <c r="N148">
+      <c r="N148" s="28">
         <v>6666666.1644430002</v>
       </c>
       <c r="O148" t="s">
@@ -10331,7 +10341,7 @@
       <c r="K149" s="26"/>
       <c r="L149" s="26"/>
       <c r="M149" s="26"/>
-      <c r="N149" s="26">
+      <c r="N149" s="28">
         <v>6666666.1644449998</v>
       </c>
       <c r="O149" s="26" t="s">
@@ -10355,7 +10365,7 @@
       <c r="K150" s="26"/>
       <c r="L150" s="26"/>
       <c r="M150" s="26"/>
-      <c r="N150" s="26">
+      <c r="N150" s="28">
         <v>6666666.164446</v>
       </c>
       <c r="O150" s="26" t="s">
@@ -10379,7 +10389,7 @@
       <c r="K151" s="26"/>
       <c r="L151" s="26"/>
       <c r="M151" s="26"/>
-      <c r="N151">
+      <c r="N151" s="28">
         <v>6666666.1646299995</v>
       </c>
       <c r="O151" t="s">
@@ -10403,7 +10413,7 @@
       <c r="K152" s="26"/>
       <c r="L152" s="26"/>
       <c r="M152" s="26"/>
-      <c r="N152">
+      <c r="N152" s="28">
         <v>6666666.1646389998</v>
       </c>
       <c r="O152" t="s">
@@ -10427,7 +10437,7 @@
       <c r="K153" s="26"/>
       <c r="L153" s="26"/>
       <c r="M153" s="26"/>
-      <c r="N153">
+      <c r="N153" s="28">
         <v>6666666.1646400001</v>
       </c>
       <c r="O153" t="s">
@@ -10451,7 +10461,7 @@
       <c r="K154" s="26"/>
       <c r="L154" s="26"/>
       <c r="M154" s="26"/>
-      <c r="N154">
+      <c r="N154" s="28">
         <v>6666666.1646410003</v>
       </c>
       <c r="O154" t="s">
@@ -10475,7 +10485,7 @@
       <c r="K155" s="26"/>
       <c r="L155" s="26"/>
       <c r="M155" s="26"/>
-      <c r="N155">
+      <c r="N155" s="28">
         <v>6666666.1646419996</v>
       </c>
       <c r="O155" t="s">
@@ -10499,7 +10509,7 @@
       <c r="K156" s="26"/>
       <c r="L156" s="26"/>
       <c r="M156" s="26"/>
-      <c r="N156">
+      <c r="N156" s="28">
         <v>6666666.1646429999</v>
       </c>
       <c r="O156" t="s">
@@ -10523,7 +10533,7 @@
       <c r="K157" s="26"/>
       <c r="L157" s="26"/>
       <c r="M157" s="26"/>
-      <c r="N157" s="26">
+      <c r="N157" s="28">
         <v>6666666.1646459997</v>
       </c>
       <c r="O157" s="26" t="s">
@@ -10547,7 +10557,7 @@
       <c r="K158" s="26"/>
       <c r="L158" s="26"/>
       <c r="M158" s="26"/>
-      <c r="N158" s="26">
+      <c r="N158" s="28">
         <v>6666666.1646469999</v>
       </c>
       <c r="O158" s="26" t="s">
@@ -10571,7 +10581,7 @@
       <c r="K159" s="26"/>
       <c r="L159" s="26"/>
       <c r="M159" s="26"/>
-      <c r="N159" s="26">
+      <c r="N159" s="28">
         <v>6666666.1646480002</v>
       </c>
       <c r="O159" s="26" t="s">
@@ -10595,7 +10605,7 @@
       <c r="K160" s="26"/>
       <c r="L160" s="26"/>
       <c r="M160" s="26"/>
-      <c r="N160" s="26">
+      <c r="N160" s="28">
         <v>6666666.1646499997</v>
       </c>
       <c r="O160" s="26" t="s">
@@ -10619,7 +10629,7 @@
       <c r="K161" s="26"/>
       <c r="L161" s="26"/>
       <c r="M161" s="26"/>
-      <c r="N161" s="26">
+      <c r="N161" s="28">
         <v>6666666.1646509999</v>
       </c>
       <c r="O161" s="26" t="s">
@@ -10643,7 +10653,7 @@
       <c r="K162" s="26"/>
       <c r="L162" s="26"/>
       <c r="M162" s="26"/>
-      <c r="N162" s="26">
+      <c r="N162" s="28">
         <v>6666666.1646560002</v>
       </c>
       <c r="O162" s="26" t="s">

</xml_diff>

<commit_message>
Finishing up in R, start of the fast parser
</commit_message>
<xml_diff>
--- a/sample_info_sorting.xlsx
+++ b/sample_info_sorting.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="542">
   <si>
     <t>sample_id</t>
   </si>
@@ -1653,9 +1653,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1848,7 +1849,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="511">
+  <cellStyleXfs count="525">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2360,8 +2361,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2435,8 +2450,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="511">
+  <cellStyles count="525">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2692,6 +2711,13 @@
     <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2947,6 +2973,13 @@
     <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5664,10 +5697,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P162"/>
+  <dimension ref="A1:T162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I133" workbookViewId="0">
-      <selection activeCell="N139" sqref="N139:N162"/>
+    <sheetView tabSelected="1" topLeftCell="I75" workbookViewId="0">
+      <selection activeCell="N99" sqref="N99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5682,10 +5715,11 @@
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28.5" customWidth="1"/>
-    <col min="16" max="16" width="21.6640625" customWidth="1"/>
+    <col min="16" max="17" width="21.6640625" customWidth="1"/>
+    <col min="18" max="18" width="15" style="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>312</v>
       </c>
@@ -5719,7 +5753,7 @@
       <c r="M1" t="s">
         <v>541</v>
       </c>
-      <c r="N1" s="26">
+      <c r="N1" s="29">
         <v>1578.78</v>
       </c>
       <c r="O1" s="26" t="s">
@@ -5728,8 +5762,17 @@
       <c r="P1" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="R1" s="32">
+        <v>1578.78</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>539</v>
+      </c>
+      <c r="T1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="B2" s="26">
         <v>200643.9</v>
       </c>
@@ -5754,7 +5797,7 @@
       <c r="K2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N2" s="26">
+      <c r="N2" s="29">
         <v>1578.8</v>
       </c>
       <c r="O2" s="26" t="s">
@@ -5763,8 +5806,17 @@
       <c r="P2" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="R2" s="32">
+        <v>1578.8</v>
+      </c>
+      <c r="S2" s="26" t="s">
+        <v>458</v>
+      </c>
+      <c r="T2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="B3" s="26">
         <v>200643.1</v>
       </c>
@@ -5789,7 +5841,7 @@
       <c r="K3" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N3" s="26">
+      <c r="N3" s="30">
         <v>200643.1</v>
       </c>
       <c r="O3" s="26" t="s">
@@ -5798,8 +5850,17 @@
       <c r="P3" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="R3" s="32">
+        <v>200643.1</v>
+      </c>
+      <c r="S3" s="26" t="s">
+        <v>451</v>
+      </c>
+      <c r="T3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="B4">
         <v>1196095.94</v>
       </c>
@@ -5824,7 +5885,7 @@
       <c r="K4" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N4" s="26">
+      <c r="N4" s="30">
         <v>200643.3</v>
       </c>
       <c r="O4" s="26" t="s">
@@ -5833,8 +5894,18 @@
       <c r="P4" s="1" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4" s="1"/>
+      <c r="R4" s="32">
+        <v>200643.3</v>
+      </c>
+      <c r="S4" s="26" t="s">
+        <v>523</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="B5">
         <v>1196095.95</v>
       </c>
@@ -5859,7 +5930,7 @@
       <c r="K5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N5" s="26">
+      <c r="N5" s="30">
         <v>200643.4</v>
       </c>
       <c r="O5" s="26" t="s">
@@ -5868,8 +5939,17 @@
       <c r="P5" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="R5" s="32">
+        <v>200643.4</v>
+      </c>
+      <c r="S5" s="26" t="s">
+        <v>530</v>
+      </c>
+      <c r="T5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="B6">
         <v>1196095.96</v>
       </c>
@@ -5894,7 +5974,7 @@
       <c r="K6" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N6" s="26">
+      <c r="N6" s="30">
         <v>200643.5</v>
       </c>
       <c r="O6" s="26" t="s">
@@ -5903,8 +5983,17 @@
       <c r="P6" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="R6" s="32">
+        <v>200643.5</v>
+      </c>
+      <c r="S6" s="26" t="s">
+        <v>532</v>
+      </c>
+      <c r="T6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="B7">
         <v>1196095.97</v>
       </c>
@@ -5929,7 +6018,7 @@
       <c r="K7" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N7" s="26">
+      <c r="N7" s="30">
         <v>200643.8</v>
       </c>
       <c r="O7" s="26" t="s">
@@ -5938,8 +6027,18 @@
       <c r="P7" s="1" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="Q7" s="1"/>
+      <c r="R7" s="32">
+        <v>200643.8</v>
+      </c>
+      <c r="S7" s="26" t="s">
+        <v>442</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
       <c r="B8">
         <v>1196095.98</v>
       </c>
@@ -5964,7 +6063,7 @@
       <c r="K8" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N8" s="26">
+      <c r="N8" s="30">
         <v>200643.9</v>
       </c>
       <c r="O8" s="26" t="s">
@@ -5973,8 +6072,17 @@
       <c r="P8" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="R8" s="32">
+        <v>200643.9</v>
+      </c>
+      <c r="S8" s="26" t="s">
+        <v>449</v>
+      </c>
+      <c r="T8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
       <c r="B9">
         <v>1196095.99</v>
       </c>
@@ -6008,8 +6116,18 @@
       <c r="P9" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="Q9" s="1"/>
+      <c r="R9" s="32">
+        <v>1196083.25</v>
+      </c>
+      <c r="S9" t="s">
+        <v>481</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="B10">
         <v>1196095.1000000001</v>
       </c>
@@ -6043,8 +6161,18 @@
       <c r="P10" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="Q10" s="1"/>
+      <c r="R10" s="32">
+        <v>1196083.26</v>
+      </c>
+      <c r="S10" t="s">
+        <v>483</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="B11">
         <v>1196095.101</v>
       </c>
@@ -6078,8 +6206,18 @@
       <c r="P11" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11" s="1"/>
+      <c r="R11" s="32">
+        <v>1196083.27</v>
+      </c>
+      <c r="S11" t="s">
+        <v>487</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="B12">
         <v>1196095.102</v>
       </c>
@@ -6113,8 +6251,18 @@
       <c r="P12" s="25" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="Q12" s="25"/>
+      <c r="R12" s="32">
+        <v>1196083.28</v>
+      </c>
+      <c r="S12" t="s">
+        <v>489</v>
+      </c>
+      <c r="T12" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
       <c r="B13">
         <v>1196095.1029999999</v>
       </c>
@@ -6148,8 +6296,18 @@
       <c r="P13" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="Q13" s="1"/>
+      <c r="R13" s="32">
+        <v>1196083.29</v>
+      </c>
+      <c r="S13" t="s">
+        <v>494</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
       <c r="B14">
         <v>1196095.1040000001</v>
       </c>
@@ -6174,7 +6332,7 @@
       <c r="K14" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N14" s="26">
+      <c r="N14" s="29">
         <v>1196083.3</v>
       </c>
       <c r="O14" s="26" t="s">
@@ -6183,8 +6341,17 @@
       <c r="P14" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="R14" s="32">
+        <v>1196083.3</v>
+      </c>
+      <c r="S14" s="26" t="s">
+        <v>540</v>
+      </c>
+      <c r="T14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
       <c r="B15">
         <v>1196095.105</v>
       </c>
@@ -6218,8 +6385,18 @@
       <c r="P15" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q15" s="1"/>
+      <c r="R15" s="32">
+        <v>1196083.31</v>
+      </c>
+      <c r="S15" t="s">
+        <v>461</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
       <c r="B16">
         <v>1196095.1059999999</v>
       </c>
@@ -6253,8 +6430,18 @@
       <c r="P16" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="17" spans="2:16">
+      <c r="Q16" s="1"/>
+      <c r="R16" s="32">
+        <v>1196083.32</v>
+      </c>
+      <c r="S16" t="s">
+        <v>463</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20">
       <c r="B17">
         <v>1196095.1070000001</v>
       </c>
@@ -6288,8 +6475,18 @@
       <c r="P17" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="18" spans="2:16">
+      <c r="Q17" s="1"/>
+      <c r="R17" s="32">
+        <v>1196083.33</v>
+      </c>
+      <c r="S17" t="s">
+        <v>464</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20">
       <c r="B18">
         <v>1196095.108</v>
       </c>
@@ -6323,8 +6520,18 @@
       <c r="P18" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="19" spans="2:16">
+      <c r="Q18" s="1"/>
+      <c r="R18" s="32">
+        <v>1196083.3400000001</v>
+      </c>
+      <c r="S18" t="s">
+        <v>475</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20">
       <c r="B19">
         <v>1196095.1089999999</v>
       </c>
@@ -6358,8 +6565,18 @@
       <c r="P19" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="20" spans="2:16">
+      <c r="Q19" s="1"/>
+      <c r="R19" s="32">
+        <v>1196083.3500000001</v>
+      </c>
+      <c r="S19" t="s">
+        <v>477</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20">
       <c r="B20">
         <v>1196095.1100000001</v>
       </c>
@@ -6393,8 +6610,18 @@
       <c r="P20" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="21" spans="2:16">
+      <c r="Q20" s="1"/>
+      <c r="R20" s="32">
+        <v>1196083.3600000001</v>
+      </c>
+      <c r="S20" t="s">
+        <v>479</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20">
       <c r="B21">
         <v>1196095.111</v>
       </c>
@@ -6428,8 +6655,18 @@
       <c r="P21" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="22" spans="2:16">
+      <c r="Q21" s="1"/>
+      <c r="R21" s="32">
+        <v>1196083.3700000001</v>
+      </c>
+      <c r="S21" t="s">
+        <v>485</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20">
       <c r="B22">
         <v>1196095.112</v>
       </c>
@@ -6463,8 +6700,18 @@
       <c r="P22" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="23" spans="2:16">
+      <c r="Q22" s="1"/>
+      <c r="R22" s="32">
+        <v>1196083.3799999999</v>
+      </c>
+      <c r="S22" t="s">
+        <v>501</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20">
       <c r="B23">
         <v>1196095.1129999999</v>
       </c>
@@ -6498,8 +6745,18 @@
       <c r="P23" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="24" spans="2:16">
+      <c r="Q23" s="1"/>
+      <c r="R23" s="32">
+        <v>1196083.3899999999</v>
+      </c>
+      <c r="S23" t="s">
+        <v>502</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20">
       <c r="B24">
         <v>1196095.1140000001</v>
       </c>
@@ -6524,7 +6781,7 @@
       <c r="K24" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N24" s="26">
+      <c r="N24" s="29">
         <v>1196083.3999999999</v>
       </c>
       <c r="O24" s="26" t="s">
@@ -6533,8 +6790,18 @@
       <c r="P24" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="25" spans="2:16">
+      <c r="Q24" s="1"/>
+      <c r="R24" s="32">
+        <v>1196083.3999999999</v>
+      </c>
+      <c r="S24" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20">
       <c r="B25">
         <v>1196095.115</v>
       </c>
@@ -6559,7 +6826,7 @@
       <c r="K25" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N25" s="26">
+      <c r="N25" s="29">
         <v>1196083.4099999999</v>
       </c>
       <c r="O25" s="26" t="s">
@@ -6568,8 +6835,18 @@
       <c r="P25" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="26" spans="2:16">
+      <c r="Q25" s="1"/>
+      <c r="R25" s="32">
+        <v>1196083.4099999999</v>
+      </c>
+      <c r="S25" s="26" t="s">
+        <v>514</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20">
       <c r="B26">
         <v>1196095.1159999999</v>
       </c>
@@ -6594,7 +6871,7 @@
       <c r="K26" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N26" s="26">
+      <c r="N26" s="29">
         <v>1196083.42</v>
       </c>
       <c r="O26" s="26" t="s">
@@ -6603,8 +6880,18 @@
       <c r="P26" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="27" spans="2:16">
+      <c r="Q26" s="1"/>
+      <c r="R26" s="32">
+        <v>1196083.42</v>
+      </c>
+      <c r="S26" s="26" t="s">
+        <v>515</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20">
       <c r="B27" s="26">
         <v>1196095.1170000001</v>
       </c>
@@ -6629,7 +6916,7 @@
       <c r="K27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N27" s="26">
+      <c r="N27" s="29">
         <v>1196083.43</v>
       </c>
       <c r="O27" s="26" t="s">
@@ -6638,8 +6925,17 @@
       <c r="P27" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="28" spans="2:16">
+      <c r="R27" s="32">
+        <v>1196083.43</v>
+      </c>
+      <c r="S27" s="26" t="s">
+        <v>526</v>
+      </c>
+      <c r="T27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20">
       <c r="B28" s="26">
         <v>1196095.118</v>
       </c>
@@ -6664,7 +6960,7 @@
       <c r="K28" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N28" s="26">
+      <c r="N28" s="29">
         <v>1196083.44</v>
       </c>
       <c r="O28" s="26" t="s">
@@ -6673,8 +6969,17 @@
       <c r="P28" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="29" spans="2:16">
+      <c r="R28" s="32">
+        <v>1196083.44</v>
+      </c>
+      <c r="S28" s="26" t="s">
+        <v>527</v>
+      </c>
+      <c r="T28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20">
       <c r="B29" s="26">
         <v>1196095.1189999999</v>
       </c>
@@ -6699,7 +7004,7 @@
       <c r="K29" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N29" s="26">
+      <c r="N29" s="29">
         <v>1196083.45</v>
       </c>
       <c r="O29" s="26" t="s">
@@ -6708,8 +7013,17 @@
       <c r="P29" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="30" spans="2:16">
+      <c r="R29" s="32">
+        <v>1196083.45</v>
+      </c>
+      <c r="S29" s="26" t="s">
+        <v>529</v>
+      </c>
+      <c r="T29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20">
       <c r="B30" s="26">
         <v>1196095.1200000001</v>
       </c>
@@ -6734,7 +7048,7 @@
       <c r="K30" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="N30" s="26">
+      <c r="N30" s="29">
         <v>1196083.46</v>
       </c>
       <c r="O30" s="26" t="s">
@@ -6743,8 +7057,17 @@
       <c r="P30" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="31" spans="2:16">
+      <c r="R30" s="32">
+        <v>1196083.46</v>
+      </c>
+      <c r="S30" s="26" t="s">
+        <v>533</v>
+      </c>
+      <c r="T30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20">
       <c r="B31" s="26">
         <v>1196095.121</v>
       </c>
@@ -6769,7 +7092,7 @@
       <c r="K31" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N31" s="26">
+      <c r="N31" s="29">
         <v>1196083.47</v>
       </c>
       <c r="O31" s="26" t="s">
@@ -6778,8 +7101,17 @@
       <c r="P31" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="32" spans="2:16">
+      <c r="R31" s="32">
+        <v>1196083.47</v>
+      </c>
+      <c r="S31" s="26" t="s">
+        <v>535</v>
+      </c>
+      <c r="T31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20">
       <c r="B32" s="26">
         <v>1196095.122</v>
       </c>
@@ -6813,8 +7145,18 @@
       <c r="P32" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="Q32" s="1"/>
+      <c r="R32" s="32">
+        <v>1196083.48</v>
+      </c>
+      <c r="S32" t="s">
+        <v>380</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
       <c r="B33" s="26">
         <v>1196095.1229999999</v>
       </c>
@@ -6848,8 +7190,18 @@
       <c r="P33" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="Q33" s="1"/>
+      <c r="R33" s="32">
+        <v>1196083.49</v>
+      </c>
+      <c r="S33" t="s">
+        <v>382</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
       <c r="B34" s="26">
         <v>1196095.1240000001</v>
       </c>
@@ -6874,7 +7226,7 @@
       <c r="K34" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="29">
         <v>1196083.5</v>
       </c>
       <c r="O34" t="s">
@@ -6883,8 +7235,18 @@
       <c r="P34" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="Q34" s="1"/>
+      <c r="R34" s="32">
+        <v>1196083.5</v>
+      </c>
+      <c r="S34" t="s">
+        <v>383</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20">
       <c r="B35" s="26">
         <v>1196095.128</v>
       </c>
@@ -6918,8 +7280,18 @@
       <c r="P35" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="Q35" s="1"/>
+      <c r="R35" s="32">
+        <v>1196083.52</v>
+      </c>
+      <c r="S35" t="s">
+        <v>394</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20">
       <c r="B36" s="26">
         <v>1196095.129</v>
       </c>
@@ -6953,8 +7325,18 @@
       <c r="P36" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="Q36" s="1"/>
+      <c r="R36" s="32">
+        <v>1196083.53</v>
+      </c>
+      <c r="S36" t="s">
+        <v>396</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20">
       <c r="B37" s="26">
         <v>1196095.1299999999</v>
       </c>
@@ -6988,8 +7370,18 @@
       <c r="P37" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="Q37" s="1"/>
+      <c r="R37" s="32">
+        <v>1196083.54</v>
+      </c>
+      <c r="S37" t="s">
+        <v>398</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20">
       <c r="B38" s="26">
         <v>1196095.1310000001</v>
       </c>
@@ -7023,8 +7415,18 @@
       <c r="P38" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="Q38" s="1"/>
+      <c r="R38" s="32">
+        <v>1196083.55</v>
+      </c>
+      <c r="S38" t="s">
+        <v>400</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20">
       <c r="B39" s="26">
         <v>1196095.1259999999</v>
       </c>
@@ -7058,8 +7460,18 @@
       <c r="P39" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="Q39" s="1"/>
+      <c r="R39" s="32">
+        <v>1196083.56</v>
+      </c>
+      <c r="S39" t="s">
+        <v>402</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
       <c r="B40" s="26">
         <v>1196095.132</v>
       </c>
@@ -7093,8 +7505,18 @@
       <c r="P40" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="Q40" s="1"/>
+      <c r="R40" s="32">
+        <v>1196083.57</v>
+      </c>
+      <c r="S40" t="s">
+        <v>404</v>
+      </c>
+      <c r="T40" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
       <c r="B41" s="26">
         <v>1196095.1329999999</v>
       </c>
@@ -7128,8 +7550,18 @@
       <c r="P41" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="Q41" s="1"/>
+      <c r="R41" s="32">
+        <v>1196083.58</v>
+      </c>
+      <c r="S41" t="s">
+        <v>406</v>
+      </c>
+      <c r="T41" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
       <c r="B42" s="26">
         <v>1196095.1340000001</v>
       </c>
@@ -7163,8 +7595,18 @@
       <c r="P42" s="25" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="Q42" s="25"/>
+      <c r="R42" s="32">
+        <v>1196083.5900000001</v>
+      </c>
+      <c r="S42" t="s">
+        <v>408</v>
+      </c>
+      <c r="T42" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20">
       <c r="B43" s="26">
         <v>1196095.135</v>
       </c>
@@ -7198,8 +7640,18 @@
       <c r="P43" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="44" spans="1:16">
+      <c r="Q43" s="1"/>
+      <c r="R43" s="32">
+        <v>1196083.6000000001</v>
+      </c>
+      <c r="S43" t="s">
+        <v>413</v>
+      </c>
+      <c r="T43" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20">
       <c r="A44" s="26"/>
       <c r="B44" s="26">
         <v>1196095.125</v>
@@ -7238,8 +7690,18 @@
       <c r="P44" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="Q44" s="1"/>
+      <c r="R44" s="32">
+        <v>1196083.6100000001</v>
+      </c>
+      <c r="S44" t="s">
+        <v>420</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20">
       <c r="A45" s="26"/>
       <c r="B45" s="26">
         <v>1196095.1270000001</v>
@@ -7278,8 +7740,18 @@
       <c r="P45" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="46" spans="1:16">
+      <c r="Q45" s="1"/>
+      <c r="R45" s="32">
+        <v>1196083.6200000001</v>
+      </c>
+      <c r="S45" t="s">
+        <v>421</v>
+      </c>
+      <c r="T45" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20">
       <c r="A46" s="26"/>
       <c r="B46" s="26">
         <v>1578.8</v>
@@ -7309,7 +7781,7 @@
       </c>
       <c r="L46" s="26"/>
       <c r="M46" s="26"/>
-      <c r="N46" s="26">
+      <c r="N46" s="29">
         <v>1196083.6299999999</v>
       </c>
       <c r="O46" s="26" t="s">
@@ -7318,8 +7790,18 @@
       <c r="P46" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="47" spans="1:16">
+      <c r="Q46" s="1"/>
+      <c r="R46" s="32">
+        <v>1196083.6299999999</v>
+      </c>
+      <c r="S46" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="T46" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20">
       <c r="A47" s="26"/>
       <c r="B47">
         <v>1196083.48</v>
@@ -7349,7 +7831,7 @@
       </c>
       <c r="L47" s="26"/>
       <c r="M47" s="26"/>
-      <c r="N47" s="26">
+      <c r="N47" s="29">
         <v>1196083.6399999999</v>
       </c>
       <c r="O47" s="26" t="s">
@@ -7358,8 +7840,18 @@
       <c r="P47" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="48" spans="1:16">
+      <c r="Q47" s="1"/>
+      <c r="R47" s="32">
+        <v>1196083.6399999999</v>
+      </c>
+      <c r="S47" s="26" t="s">
+        <v>433</v>
+      </c>
+      <c r="T47" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20">
       <c r="A48" s="26"/>
       <c r="B48">
         <v>1196083.49</v>
@@ -7389,7 +7881,7 @@
       </c>
       <c r="L48" s="26"/>
       <c r="M48" s="26"/>
-      <c r="N48" s="26">
+      <c r="N48" s="29">
         <v>1196083.6499999999</v>
       </c>
       <c r="O48" s="26" t="s">
@@ -7398,8 +7890,18 @@
       <c r="P48" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="49" spans="1:16">
+      <c r="Q48" s="1"/>
+      <c r="R48" s="32">
+        <v>1196083.6499999999</v>
+      </c>
+      <c r="S48" s="26" t="s">
+        <v>434</v>
+      </c>
+      <c r="T48" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20">
       <c r="A49" s="26"/>
       <c r="B49">
         <v>1196083.5</v>
@@ -7429,7 +7931,7 @@
       </c>
       <c r="L49" s="26"/>
       <c r="M49" s="26"/>
-      <c r="N49" s="26">
+      <c r="N49" s="29">
         <v>1196083.6599999999</v>
       </c>
       <c r="O49" s="26" t="s">
@@ -7438,8 +7940,17 @@
       <c r="P49" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="50" spans="1:16">
+      <c r="R49" s="32">
+        <v>1196083.6599999999</v>
+      </c>
+      <c r="S49" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="T49" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20">
       <c r="A50" s="26"/>
       <c r="B50">
         <v>1196083.52</v>
@@ -7469,7 +7980,7 @@
       </c>
       <c r="L50" s="26"/>
       <c r="M50" s="26"/>
-      <c r="N50" s="26">
+      <c r="N50" s="29">
         <v>1196083.67</v>
       </c>
       <c r="O50" s="26" t="s">
@@ -7478,8 +7989,17 @@
       <c r="P50" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="51" spans="1:16">
+      <c r="R50" s="32">
+        <v>1196083.67</v>
+      </c>
+      <c r="S50" s="26" t="s">
+        <v>445</v>
+      </c>
+      <c r="T50" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20">
       <c r="A51" s="26"/>
       <c r="B51">
         <v>1196083.53</v>
@@ -7509,7 +8029,7 @@
       </c>
       <c r="L51" s="26"/>
       <c r="M51" s="26"/>
-      <c r="N51" s="26">
+      <c r="N51" s="29">
         <v>1196083.68</v>
       </c>
       <c r="O51" s="26" t="s">
@@ -7518,8 +8038,17 @@
       <c r="P51" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="52" spans="1:16">
+      <c r="R51" s="32">
+        <v>1196083.68</v>
+      </c>
+      <c r="S51" s="26" t="s">
+        <v>446</v>
+      </c>
+      <c r="T51" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20">
       <c r="A52" s="26"/>
       <c r="B52">
         <v>1196083.54</v>
@@ -7549,7 +8078,7 @@
       </c>
       <c r="L52" s="26"/>
       <c r="M52" s="26"/>
-      <c r="N52" s="26">
+      <c r="N52" s="29">
         <v>1196083.69</v>
       </c>
       <c r="O52" s="26" t="s">
@@ -7558,8 +8087,17 @@
       <c r="P52" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="53" spans="1:16">
+      <c r="R52" s="32">
+        <v>1196083.69</v>
+      </c>
+      <c r="S52" s="26" t="s">
+        <v>448</v>
+      </c>
+      <c r="T52" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20">
       <c r="A53" s="26"/>
       <c r="B53">
         <v>1196083.55</v>
@@ -7589,7 +8127,7 @@
       </c>
       <c r="L53" s="26"/>
       <c r="M53" s="26"/>
-      <c r="N53" s="26">
+      <c r="N53" s="29">
         <v>1196083.7</v>
       </c>
       <c r="O53" s="26" t="s">
@@ -7598,8 +8136,17 @@
       <c r="P53" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="54" spans="1:16">
+      <c r="R53" s="32">
+        <v>1196083.7</v>
+      </c>
+      <c r="S53" s="26" t="s">
+        <v>452</v>
+      </c>
+      <c r="T53" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20">
       <c r="A54" s="26"/>
       <c r="B54">
         <v>1196083.56</v>
@@ -7629,7 +8176,7 @@
       </c>
       <c r="L54" s="26"/>
       <c r="M54" s="26"/>
-      <c r="N54" s="26">
+      <c r="N54" s="29">
         <v>1196083.71</v>
       </c>
       <c r="O54" s="26" t="s">
@@ -7638,8 +8185,17 @@
       <c r="P54" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="55" spans="1:16">
+      <c r="R54" s="32">
+        <v>1196083.71</v>
+      </c>
+      <c r="S54" s="26" t="s">
+        <v>454</v>
+      </c>
+      <c r="T54" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20">
       <c r="A55" s="26"/>
       <c r="B55">
         <v>1196083.57</v>
@@ -7669,7 +8225,7 @@
       </c>
       <c r="L55" s="26"/>
       <c r="M55" s="26"/>
-      <c r="N55">
+      <c r="N55" s="26">
         <v>1196095.1000000001</v>
       </c>
       <c r="O55" t="s">
@@ -7678,8 +8234,18 @@
       <c r="P55" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="56" spans="1:16">
+      <c r="Q55" s="1"/>
+      <c r="R55" s="32">
+        <v>1196095.1000000001</v>
+      </c>
+      <c r="S55" t="s">
+        <v>389</v>
+      </c>
+      <c r="T55" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20">
       <c r="A56" s="26"/>
       <c r="B56">
         <v>1196083.58</v>
@@ -7718,8 +8284,18 @@
       <c r="P56" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="57" spans="1:16">
+      <c r="Q56" s="1"/>
+      <c r="R56" s="32">
+        <v>1196095.101</v>
+      </c>
+      <c r="S56" t="s">
+        <v>390</v>
+      </c>
+      <c r="T56" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20">
       <c r="A57" s="26"/>
       <c r="B57">
         <v>1196083.5900000001</v>
@@ -7758,8 +8334,18 @@
       <c r="P57" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="58" spans="1:16">
+      <c r="Q57" s="1"/>
+      <c r="R57" s="32">
+        <v>1196095.102</v>
+      </c>
+      <c r="S57" t="s">
+        <v>391</v>
+      </c>
+      <c r="T57" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20">
       <c r="A58" s="26"/>
       <c r="B58">
         <v>1196083.6000000001</v>
@@ -7798,8 +8384,18 @@
       <c r="P58" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="59" spans="1:16">
+      <c r="Q58" s="1"/>
+      <c r="R58" s="32">
+        <v>1196095.1029999999</v>
+      </c>
+      <c r="S58" t="s">
+        <v>392</v>
+      </c>
+      <c r="T58" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20">
       <c r="A59" s="26"/>
       <c r="B59">
         <v>1196083.6100000001</v>
@@ -7838,8 +8434,18 @@
       <c r="P59" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="60" spans="1:16">
+      <c r="Q59" s="1"/>
+      <c r="R59" s="32">
+        <v>1196095.1040000001</v>
+      </c>
+      <c r="S59" t="s">
+        <v>393</v>
+      </c>
+      <c r="T59" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20">
       <c r="A60" s="26"/>
       <c r="B60">
         <v>1196083.6200000001</v>
@@ -7878,8 +8484,18 @@
       <c r="P60" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="61" spans="1:16">
+      <c r="Q60" s="1"/>
+      <c r="R60" s="32">
+        <v>1196095.105</v>
+      </c>
+      <c r="S60" t="s">
+        <v>395</v>
+      </c>
+      <c r="T60" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20">
       <c r="A61" s="26"/>
       <c r="B61" s="26">
         <v>1196083.6299999999</v>
@@ -7918,8 +8534,18 @@
       <c r="P61" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="62" spans="1:16">
+      <c r="Q61" s="1"/>
+      <c r="R61" s="32">
+        <v>1196095.1059999999</v>
+      </c>
+      <c r="S61" t="s">
+        <v>397</v>
+      </c>
+      <c r="T61" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20">
       <c r="A62" s="26"/>
       <c r="B62" s="26">
         <v>1196083.6399999999</v>
@@ -7958,8 +8584,18 @@
       <c r="P62" s="25" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="63" spans="1:16">
+      <c r="Q62" s="25"/>
+      <c r="R62" s="32">
+        <v>1196095.1070000001</v>
+      </c>
+      <c r="S62" t="s">
+        <v>399</v>
+      </c>
+      <c r="T62" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20">
       <c r="A63" s="26"/>
       <c r="B63" s="26">
         <v>1196083.6499999999</v>
@@ -7998,8 +8634,18 @@
       <c r="P63" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="64" spans="1:16">
+      <c r="Q63" s="1"/>
+      <c r="R63" s="32">
+        <v>1196095.108</v>
+      </c>
+      <c r="S63" t="s">
+        <v>401</v>
+      </c>
+      <c r="T63" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20">
       <c r="A64" s="26"/>
       <c r="B64" s="26">
         <v>1196083.67</v>
@@ -8038,8 +8684,18 @@
       <c r="P64" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="65" spans="1:16">
+      <c r="Q64" s="1"/>
+      <c r="R64" s="32">
+        <v>1196095.1089999999</v>
+      </c>
+      <c r="S64" t="s">
+        <v>403</v>
+      </c>
+      <c r="T64" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20">
       <c r="A65" s="26"/>
       <c r="B65" s="26">
         <v>1196083.68</v>
@@ -8069,7 +8725,7 @@
       </c>
       <c r="L65" s="26"/>
       <c r="M65" s="26"/>
-      <c r="N65">
+      <c r="N65" s="26">
         <v>1196095.1100000001</v>
       </c>
       <c r="O65" t="s">
@@ -8078,8 +8734,18 @@
       <c r="P65" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="66" spans="1:16">
+      <c r="Q65" s="1"/>
+      <c r="R65" s="32">
+        <v>1196095.1100000001</v>
+      </c>
+      <c r="S65" t="s">
+        <v>405</v>
+      </c>
+      <c r="T65" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
       <c r="A66" s="26"/>
       <c r="B66" s="26">
         <v>1196083.69</v>
@@ -8118,8 +8784,18 @@
       <c r="P66" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="67" spans="1:16">
+      <c r="Q66" s="1"/>
+      <c r="R66" s="32">
+        <v>1196095.111</v>
+      </c>
+      <c r="S66" t="s">
+        <v>407</v>
+      </c>
+      <c r="T66" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20">
       <c r="A67" s="26"/>
       <c r="B67" s="26">
         <v>1196083.7</v>
@@ -8158,8 +8834,18 @@
       <c r="P67" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="68" spans="1:16">
+      <c r="Q67" s="1"/>
+      <c r="R67" s="32">
+        <v>1196095.112</v>
+      </c>
+      <c r="S67" t="s">
+        <v>409</v>
+      </c>
+      <c r="T67" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
       <c r="A68" s="26"/>
       <c r="B68" s="26">
         <v>1196083.71</v>
@@ -8198,8 +8884,18 @@
       <c r="P68" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="69" spans="1:16">
+      <c r="Q68" s="1"/>
+      <c r="R68" s="32">
+        <v>1196095.1129999999</v>
+      </c>
+      <c r="S68" t="s">
+        <v>410</v>
+      </c>
+      <c r="T68" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
       <c r="A69" s="26"/>
       <c r="B69" s="26">
         <v>1196083.6599999999</v>
@@ -8238,8 +8934,18 @@
       <c r="P69" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="70" spans="1:16">
+      <c r="Q69" s="1"/>
+      <c r="R69" s="32">
+        <v>1196095.1140000001</v>
+      </c>
+      <c r="S69" t="s">
+        <v>412</v>
+      </c>
+      <c r="T69" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20">
       <c r="A70" s="26"/>
       <c r="B70" s="28">
         <v>6666666.1646299995</v>
@@ -8278,8 +8984,18 @@
       <c r="P70" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="71" spans="1:16">
+      <c r="Q70" s="1"/>
+      <c r="R70" s="32">
+        <v>1196095.115</v>
+      </c>
+      <c r="S70" t="s">
+        <v>416</v>
+      </c>
+      <c r="T70" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20">
       <c r="A71" s="26"/>
       <c r="B71" s="28">
         <v>6666666.1646389998</v>
@@ -8318,8 +9034,18 @@
       <c r="P71" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="72" spans="1:16">
+      <c r="Q71" s="1"/>
+      <c r="R71" s="32">
+        <v>1196095.1159999999</v>
+      </c>
+      <c r="S71" t="s">
+        <v>419</v>
+      </c>
+      <c r="T71" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20">
       <c r="A72" s="26"/>
       <c r="B72" s="28">
         <v>6666666.1646400001</v>
@@ -8358,8 +9084,18 @@
       <c r="P72" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="73" spans="1:16">
+      <c r="Q72" s="1"/>
+      <c r="R72" s="32">
+        <v>1196095.1170000001</v>
+      </c>
+      <c r="S72" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="T72" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20">
       <c r="A73" s="26"/>
       <c r="B73" s="28">
         <v>6666666.1646410003</v>
@@ -8398,8 +9134,18 @@
       <c r="P73" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="74" spans="1:16">
+      <c r="Q73" s="1"/>
+      <c r="R73" s="32">
+        <v>1196095.118</v>
+      </c>
+      <c r="S73" s="26" t="s">
+        <v>423</v>
+      </c>
+      <c r="T73" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20">
       <c r="A74" s="26"/>
       <c r="B74" s="28">
         <v>6666666.1646419996</v>
@@ -8438,8 +9184,18 @@
       <c r="P74" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="75" spans="1:16">
+      <c r="Q74" s="1"/>
+      <c r="R74" s="32">
+        <v>1196095.1189999999</v>
+      </c>
+      <c r="S74" s="26" t="s">
+        <v>424</v>
+      </c>
+      <c r="T74" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20">
       <c r="A75" s="26"/>
       <c r="B75" s="28">
         <v>6666666.1646429999</v>
@@ -8478,8 +9234,18 @@
       <c r="P75" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="76" spans="1:16">
+      <c r="Q75" s="1"/>
+      <c r="R75" s="32">
+        <v>1196095.1200000001</v>
+      </c>
+      <c r="S75" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="T75" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20">
       <c r="A76" s="26"/>
       <c r="B76" s="28">
         <v>6666666.1646459997</v>
@@ -8518,8 +9284,18 @@
       <c r="P76" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="77" spans="1:16">
+      <c r="Q76" s="1"/>
+      <c r="R76" s="32">
+        <v>1196095.121</v>
+      </c>
+      <c r="S76" s="26" t="s">
+        <v>428</v>
+      </c>
+      <c r="T76" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20">
       <c r="A77" s="26"/>
       <c r="B77" s="28">
         <v>6666666.1646469999</v>
@@ -8558,8 +9334,18 @@
       <c r="P77" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="78" spans="1:16">
+      <c r="Q77" s="1"/>
+      <c r="R77" s="32">
+        <v>1196095.122</v>
+      </c>
+      <c r="S77" s="26" t="s">
+        <v>429</v>
+      </c>
+      <c r="T77" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20">
       <c r="A78" s="26"/>
       <c r="B78" s="28">
         <v>6666666.1646480002</v>
@@ -8598,8 +9384,18 @@
       <c r="P78" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="79" spans="1:16">
+      <c r="Q78" s="1"/>
+      <c r="R78" s="32">
+        <v>1196095.1229999999</v>
+      </c>
+      <c r="S78" s="26" t="s">
+        <v>432</v>
+      </c>
+      <c r="T78" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20">
       <c r="A79" s="26"/>
       <c r="B79" s="28">
         <v>6666666.1646499997</v>
@@ -8638,8 +9434,18 @@
       <c r="P79" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="80" spans="1:16">
+      <c r="Q79" s="1"/>
+      <c r="R79" s="32">
+        <v>1196095.1240000001</v>
+      </c>
+      <c r="S79" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="T79" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20">
       <c r="A80" s="26"/>
       <c r="B80" s="28">
         <v>6666666.1646509999</v>
@@ -8678,8 +9484,17 @@
       <c r="P80" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="81" spans="1:16">
+      <c r="R80" s="32">
+        <v>1196095.125</v>
+      </c>
+      <c r="S80" s="26" t="s">
+        <v>456</v>
+      </c>
+      <c r="T80" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20">
       <c r="A81" s="26"/>
       <c r="B81" s="28">
         <v>6666666.1646560002</v>
@@ -8718,8 +9533,18 @@
       <c r="P81" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="82" spans="1:16">
+      <c r="Q81" s="1"/>
+      <c r="R81" s="32">
+        <v>1196095.1259999999</v>
+      </c>
+      <c r="S81" s="26" t="s">
+        <v>441</v>
+      </c>
+      <c r="T81" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20">
       <c r="A82" s="26"/>
       <c r="B82" s="26"/>
       <c r="C82" s="26"/>
@@ -8742,8 +9567,17 @@
       <c r="P82" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="83" spans="1:16">
+      <c r="R82" s="32">
+        <v>1196095.1270000001</v>
+      </c>
+      <c r="S82" s="26" t="s">
+        <v>457</v>
+      </c>
+      <c r="T82" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20">
       <c r="A83" s="26"/>
       <c r="B83" s="26"/>
       <c r="C83" s="26"/>
@@ -8766,8 +9600,18 @@
       <c r="P83" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="84" spans="1:16">
+      <c r="Q83" s="1"/>
+      <c r="R83" s="32">
+        <v>1196095.128</v>
+      </c>
+      <c r="S83" s="26" t="s">
+        <v>437</v>
+      </c>
+      <c r="T83" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20">
       <c r="A84" s="26"/>
       <c r="B84" s="26"/>
       <c r="C84" s="26"/>
@@ -8790,8 +9634,18 @@
       <c r="P84" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="85" spans="1:16">
+      <c r="Q84" s="1"/>
+      <c r="R84" s="32">
+        <v>1196095.129</v>
+      </c>
+      <c r="S84" s="26" t="s">
+        <v>438</v>
+      </c>
+      <c r="T84" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20">
       <c r="A85" s="26"/>
       <c r="B85" s="26"/>
       <c r="C85" s="26"/>
@@ -8814,8 +9668,18 @@
       <c r="P85" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="86" spans="1:16">
+      <c r="Q85" s="1"/>
+      <c r="R85" s="32">
+        <v>1196095.1299999999</v>
+      </c>
+      <c r="S85" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="T85" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20">
       <c r="A86" s="26"/>
       <c r="B86" s="26"/>
       <c r="C86" s="26"/>
@@ -8838,8 +9702,18 @@
       <c r="P86" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="87" spans="1:16">
+      <c r="Q86" s="1"/>
+      <c r="R86" s="32">
+        <v>1196095.1310000001</v>
+      </c>
+      <c r="S86" s="26" t="s">
+        <v>440</v>
+      </c>
+      <c r="T86" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20">
       <c r="A87" s="26"/>
       <c r="B87" s="26"/>
       <c r="C87" s="26"/>
@@ -8862,8 +9736,18 @@
       <c r="P87" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="88" spans="1:16">
+      <c r="Q87" s="1"/>
+      <c r="R87" s="32">
+        <v>1196095.132</v>
+      </c>
+      <c r="S87" s="26" t="s">
+        <v>443</v>
+      </c>
+      <c r="T87" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20">
       <c r="A88" s="26"/>
       <c r="B88" s="26"/>
       <c r="C88" s="26"/>
@@ -8886,8 +9770,17 @@
       <c r="P88" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="89" spans="1:16">
+      <c r="R88" s="32">
+        <v>1196095.1329999999</v>
+      </c>
+      <c r="S88" s="26" t="s">
+        <v>444</v>
+      </c>
+      <c r="T88" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20">
       <c r="A89" s="26"/>
       <c r="B89" s="26"/>
       <c r="C89" s="26"/>
@@ -8910,8 +9803,17 @@
       <c r="P89" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="90" spans="1:16">
+      <c r="R89" s="32">
+        <v>1196095.1340000001</v>
+      </c>
+      <c r="S89" s="26" t="s">
+        <v>447</v>
+      </c>
+      <c r="T89" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20">
       <c r="A90" s="26"/>
       <c r="B90" s="26"/>
       <c r="C90" s="26"/>
@@ -8934,8 +9836,17 @@
       <c r="P90" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="91" spans="1:16">
+      <c r="R90" s="32">
+        <v>1196095.135</v>
+      </c>
+      <c r="S90" s="26" t="s">
+        <v>450</v>
+      </c>
+      <c r="T90" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20">
       <c r="A91" s="26"/>
       <c r="B91" s="26"/>
       <c r="C91" s="26"/>
@@ -8958,8 +9869,18 @@
       <c r="P91" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="92" spans="1:16">
+      <c r="Q91" s="1"/>
+      <c r="R91" s="32">
+        <v>1196095.51</v>
+      </c>
+      <c r="S91" t="s">
+        <v>467</v>
+      </c>
+      <c r="T91" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20">
       <c r="A92" s="26"/>
       <c r="B92" s="26"/>
       <c r="C92" s="26"/>
@@ -8982,8 +9903,18 @@
       <c r="P92" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="93" spans="1:16">
+      <c r="Q92" s="1"/>
+      <c r="R92" s="32">
+        <v>1196095.53</v>
+      </c>
+      <c r="S92" t="s">
+        <v>470</v>
+      </c>
+      <c r="T92" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20">
       <c r="A93" s="26"/>
       <c r="B93" s="26"/>
       <c r="C93" s="26"/>
@@ -9006,8 +9937,18 @@
       <c r="P93" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="94" spans="1:16">
+      <c r="Q93" s="1"/>
+      <c r="R93" s="32">
+        <v>1196095.54</v>
+      </c>
+      <c r="S93" t="s">
+        <v>471</v>
+      </c>
+      <c r="T93" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20">
       <c r="A94" s="26"/>
       <c r="B94" s="26"/>
       <c r="C94" s="26"/>
@@ -9030,8 +9971,18 @@
       <c r="P94" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="95" spans="1:16">
+      <c r="Q94" s="1"/>
+      <c r="R94" s="32">
+        <v>1196095.55</v>
+      </c>
+      <c r="S94" t="s">
+        <v>472</v>
+      </c>
+      <c r="T94" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20">
       <c r="A95" s="26"/>
       <c r="B95" s="26"/>
       <c r="C95" s="26"/>
@@ -9054,8 +10005,18 @@
       <c r="P95" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="96" spans="1:16">
+      <c r="Q95" s="1"/>
+      <c r="R95" s="32">
+        <v>1196095.56</v>
+      </c>
+      <c r="S95" t="s">
+        <v>473</v>
+      </c>
+      <c r="T95" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20">
       <c r="A96" s="26"/>
       <c r="B96" s="26"/>
       <c r="C96" s="26"/>
@@ -9078,8 +10039,18 @@
       <c r="P96" s="25" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="97" spans="1:16">
+      <c r="Q96" s="25"/>
+      <c r="R96" s="32">
+        <v>1196095.57</v>
+      </c>
+      <c r="S96" t="s">
+        <v>480</v>
+      </c>
+      <c r="T96" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20">
       <c r="A97" s="26"/>
       <c r="B97" s="26"/>
       <c r="C97" s="26"/>
@@ -9102,8 +10073,18 @@
       <c r="P97" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="98" spans="1:16">
+      <c r="Q97" s="1"/>
+      <c r="R97" s="32">
+        <v>1196095.58</v>
+      </c>
+      <c r="S97" t="s">
+        <v>482</v>
+      </c>
+      <c r="T97" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20">
       <c r="A98" s="26"/>
       <c r="B98" s="26"/>
       <c r="C98" s="26"/>
@@ -9126,8 +10107,18 @@
       <c r="P98" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="99" spans="1:16">
+      <c r="Q98" s="1"/>
+      <c r="R98" s="32">
+        <v>1196095.5900000001</v>
+      </c>
+      <c r="S98" t="s">
+        <v>486</v>
+      </c>
+      <c r="T98" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20">
       <c r="A99" s="26"/>
       <c r="B99" s="26"/>
       <c r="C99" s="26"/>
@@ -9141,7 +10132,7 @@
       <c r="K99" s="26"/>
       <c r="L99" s="26"/>
       <c r="M99" s="26"/>
-      <c r="N99">
+      <c r="N99" s="29">
         <v>1196095.6000000001</v>
       </c>
       <c r="O99" t="s">
@@ -9150,8 +10141,18 @@
       <c r="P99" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="100" spans="1:16">
+      <c r="Q99" s="1"/>
+      <c r="R99" s="32">
+        <v>1196095.6000000001</v>
+      </c>
+      <c r="S99" t="s">
+        <v>488</v>
+      </c>
+      <c r="T99" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20">
       <c r="A100" s="26"/>
       <c r="B100" s="26"/>
       <c r="C100" s="26"/>
@@ -9174,8 +10175,18 @@
       <c r="P100" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="101" spans="1:16">
+      <c r="Q100" s="1"/>
+      <c r="R100" s="32">
+        <v>1196095.6100000001</v>
+      </c>
+      <c r="S100" t="s">
+        <v>490</v>
+      </c>
+      <c r="T100" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20">
       <c r="A101" s="26"/>
       <c r="B101" s="26"/>
       <c r="C101" s="26"/>
@@ -9198,8 +10209,18 @@
       <c r="P101" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="102" spans="1:16">
+      <c r="Q101" s="1"/>
+      <c r="R101" s="32">
+        <v>1196095.6200000001</v>
+      </c>
+      <c r="S101" t="s">
+        <v>491</v>
+      </c>
+      <c r="T101" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20">
       <c r="A102" s="26"/>
       <c r="B102" s="26"/>
       <c r="C102" s="26"/>
@@ -9222,8 +10243,18 @@
       <c r="P102" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="103" spans="1:16">
+      <c r="Q102" s="1"/>
+      <c r="R102" s="32">
+        <v>1196095.6299999999</v>
+      </c>
+      <c r="S102" t="s">
+        <v>493</v>
+      </c>
+      <c r="T102" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20">
       <c r="A103" s="26"/>
       <c r="B103" s="26"/>
       <c r="C103" s="26"/>
@@ -9246,8 +10277,18 @@
       <c r="P103" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="104" spans="1:16">
+      <c r="Q103" s="1"/>
+      <c r="R103" s="32">
+        <v>1196095.6399999999</v>
+      </c>
+      <c r="S103" t="s">
+        <v>497</v>
+      </c>
+      <c r="T103" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20">
       <c r="A104" s="26"/>
       <c r="B104" s="26"/>
       <c r="C104" s="26"/>
@@ -9261,7 +10302,7 @@
       <c r="K104" s="26"/>
       <c r="L104" s="26"/>
       <c r="M104" s="26"/>
-      <c r="N104" s="26">
+      <c r="N104" s="29">
         <v>1196095.6499999999</v>
       </c>
       <c r="O104" s="26" t="s">
@@ -9270,8 +10311,18 @@
       <c r="P104" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="105" spans="1:16">
+      <c r="Q104" s="1"/>
+      <c r="R104" s="32">
+        <v>1196095.6499999999</v>
+      </c>
+      <c r="S104" s="26" t="s">
+        <v>509</v>
+      </c>
+      <c r="T104" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20">
       <c r="A105" s="26"/>
       <c r="B105" s="26"/>
       <c r="C105" s="26"/>
@@ -9285,7 +10336,7 @@
       <c r="K105" s="26"/>
       <c r="L105" s="26"/>
       <c r="M105" s="26"/>
-      <c r="N105" s="26">
+      <c r="N105" s="29">
         <v>1196095.6599999999</v>
       </c>
       <c r="O105" s="26" t="s">
@@ -9294,8 +10345,18 @@
       <c r="P105" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="106" spans="1:16">
+      <c r="Q105" s="1"/>
+      <c r="R105" s="32">
+        <v>1196095.6599999999</v>
+      </c>
+      <c r="S105" s="26" t="s">
+        <v>510</v>
+      </c>
+      <c r="T105" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20">
       <c r="A106" s="26"/>
       <c r="B106" s="26"/>
       <c r="C106" s="26"/>
@@ -9309,7 +10370,7 @@
       <c r="K106" s="26"/>
       <c r="L106" s="26"/>
       <c r="M106" s="26"/>
-      <c r="N106" s="26">
+      <c r="N106" s="29">
         <v>1196095.67</v>
       </c>
       <c r="O106" s="26" t="s">
@@ -9318,8 +10379,18 @@
       <c r="P106" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="107" spans="1:16">
+      <c r="Q106" s="1"/>
+      <c r="R106" s="32">
+        <v>1196095.67</v>
+      </c>
+      <c r="S106" s="26" t="s">
+        <v>513</v>
+      </c>
+      <c r="T106" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20">
       <c r="A107" s="26"/>
       <c r="B107" s="26"/>
       <c r="C107" s="26"/>
@@ -9333,7 +10404,7 @@
       <c r="K107" s="26"/>
       <c r="L107" s="26"/>
       <c r="M107" s="26"/>
-      <c r="N107" s="26">
+      <c r="N107" s="29">
         <v>1196095.68</v>
       </c>
       <c r="O107" s="26" t="s">
@@ -9342,8 +10413,17 @@
       <c r="P107" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="108" spans="1:16">
+      <c r="R107" s="32">
+        <v>1196095.68</v>
+      </c>
+      <c r="S107" s="26" t="s">
+        <v>537</v>
+      </c>
+      <c r="T107" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20">
       <c r="A108" s="26"/>
       <c r="B108" s="26"/>
       <c r="C108" s="26"/>
@@ -9357,7 +10437,7 @@
       <c r="K108" s="26"/>
       <c r="L108" s="26"/>
       <c r="M108" s="26"/>
-      <c r="N108" s="26">
+      <c r="N108" s="29">
         <v>1196095.69</v>
       </c>
       <c r="O108" s="26" t="s">
@@ -9366,8 +10446,18 @@
       <c r="P108" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="109" spans="1:16">
+      <c r="Q108" s="1"/>
+      <c r="R108" s="32">
+        <v>1196095.69</v>
+      </c>
+      <c r="S108" s="26" t="s">
+        <v>522</v>
+      </c>
+      <c r="T108" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20">
       <c r="A109" s="26"/>
       <c r="B109" s="26"/>
       <c r="C109" s="26"/>
@@ -9381,7 +10471,7 @@
       <c r="K109" s="26"/>
       <c r="L109" s="26"/>
       <c r="M109" s="26"/>
-      <c r="N109">
+      <c r="N109" s="29">
         <v>1196095.7</v>
       </c>
       <c r="O109" t="s">
@@ -9390,8 +10480,18 @@
       <c r="P109" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="110" spans="1:16">
+      <c r="Q109" s="1"/>
+      <c r="R109" s="32">
+        <v>1196095.7</v>
+      </c>
+      <c r="S109" t="s">
+        <v>460</v>
+      </c>
+      <c r="T109" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20">
       <c r="A110" s="26"/>
       <c r="B110" s="26"/>
       <c r="C110" s="26"/>
@@ -9414,8 +10514,18 @@
       <c r="P110" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="111" spans="1:16">
+      <c r="Q110" s="1"/>
+      <c r="R110" s="32">
+        <v>1196095.71</v>
+      </c>
+      <c r="S110" t="s">
+        <v>462</v>
+      </c>
+      <c r="T110" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20">
       <c r="A111" s="26"/>
       <c r="B111" s="26"/>
       <c r="C111" s="26"/>
@@ -9438,8 +10548,18 @@
       <c r="P111" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="112" spans="1:16">
+      <c r="Q111" s="1"/>
+      <c r="R111" s="32">
+        <v>1196095.72</v>
+      </c>
+      <c r="S111" t="s">
+        <v>465</v>
+      </c>
+      <c r="T111" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20">
       <c r="A112" s="26"/>
       <c r="B112" s="26"/>
       <c r="C112" s="26"/>
@@ -9462,8 +10582,18 @@
       <c r="P112" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="113" spans="1:16">
+      <c r="Q112" s="1"/>
+      <c r="R112" s="32">
+        <v>1196095.73</v>
+      </c>
+      <c r="S112" t="s">
+        <v>466</v>
+      </c>
+      <c r="T112" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20">
       <c r="A113" s="26"/>
       <c r="B113" s="26"/>
       <c r="C113" s="26"/>
@@ -9486,8 +10616,18 @@
       <c r="P113" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="114" spans="1:16">
+      <c r="Q113" s="1"/>
+      <c r="R113" s="32">
+        <v>1196095.74</v>
+      </c>
+      <c r="S113" t="s">
+        <v>468</v>
+      </c>
+      <c r="T113" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20">
       <c r="A114" s="26"/>
       <c r="B114" s="26"/>
       <c r="C114" s="26"/>
@@ -9510,8 +10650,18 @@
       <c r="P114" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="115" spans="1:16">
+      <c r="Q114" s="1"/>
+      <c r="R114" s="32">
+        <v>1196095.75</v>
+      </c>
+      <c r="S114" t="s">
+        <v>474</v>
+      </c>
+      <c r="T114" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20">
       <c r="A115" s="26"/>
       <c r="B115" s="26"/>
       <c r="C115" s="26"/>
@@ -9534,8 +10684,18 @@
       <c r="P115" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="116" spans="1:16">
+      <c r="Q115" s="1"/>
+      <c r="R115" s="32">
+        <v>1196095.76</v>
+      </c>
+      <c r="S115" t="s">
+        <v>476</v>
+      </c>
+      <c r="T115" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20">
       <c r="A116" s="26"/>
       <c r="B116" s="26"/>
       <c r="C116" s="26"/>
@@ -9558,8 +10718,18 @@
       <c r="P116" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="117" spans="1:16">
+      <c r="Q116" s="1"/>
+      <c r="R116" s="32">
+        <v>1196095.77</v>
+      </c>
+      <c r="S116" t="s">
+        <v>478</v>
+      </c>
+      <c r="T116" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20">
       <c r="A117" s="26"/>
       <c r="B117" s="26"/>
       <c r="C117" s="26"/>
@@ -9582,8 +10752,18 @@
       <c r="P117" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="118" spans="1:16">
+      <c r="Q117" s="1"/>
+      <c r="R117" s="32">
+        <v>1196095.78</v>
+      </c>
+      <c r="S117" t="s">
+        <v>484</v>
+      </c>
+      <c r="T117" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20">
       <c r="A118" s="26"/>
       <c r="B118" s="26"/>
       <c r="C118" s="26"/>
@@ -9606,8 +10786,18 @@
       <c r="P118" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="119" spans="1:16">
+      <c r="Q118" s="1"/>
+      <c r="R118" s="32">
+        <v>1196095.79</v>
+      </c>
+      <c r="S118" t="s">
+        <v>500</v>
+      </c>
+      <c r="T118" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20">
       <c r="A119" s="26"/>
       <c r="B119" s="26"/>
       <c r="C119" s="26"/>
@@ -9621,7 +10811,7 @@
       <c r="K119" s="26"/>
       <c r="L119" s="26"/>
       <c r="M119" s="26"/>
-      <c r="N119" s="26">
+      <c r="N119" s="29">
         <v>1196095.8</v>
       </c>
       <c r="O119" s="26" t="s">
@@ -9630,8 +10820,18 @@
       <c r="P119" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="120" spans="1:16">
+      <c r="Q119" s="1"/>
+      <c r="R119" s="32">
+        <v>1196095.8</v>
+      </c>
+      <c r="S119" s="26" t="s">
+        <v>503</v>
+      </c>
+      <c r="T119" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20">
       <c r="A120" s="26"/>
       <c r="B120" s="26"/>
       <c r="C120" s="26"/>
@@ -9645,7 +10845,7 @@
       <c r="K120" s="26"/>
       <c r="L120" s="26"/>
       <c r="M120" s="26"/>
-      <c r="N120" s="26">
+      <c r="N120" s="29">
         <v>1196095.81</v>
       </c>
       <c r="O120" s="26" t="s">
@@ -9654,8 +10854,18 @@
       <c r="P120" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="121" spans="1:16">
+      <c r="Q120" s="1"/>
+      <c r="R120" s="32">
+        <v>1196095.81</v>
+      </c>
+      <c r="S120" s="26" t="s">
+        <v>504</v>
+      </c>
+      <c r="T120" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20">
       <c r="A121" s="26"/>
       <c r="B121" s="26"/>
       <c r="C121" s="26"/>
@@ -9669,7 +10879,7 @@
       <c r="K121" s="26"/>
       <c r="L121" s="26"/>
       <c r="M121" s="26"/>
-      <c r="N121" s="26">
+      <c r="N121" s="29">
         <v>1196095.82</v>
       </c>
       <c r="O121" s="26" t="s">
@@ -9678,8 +10888,18 @@
       <c r="P121" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="122" spans="1:16">
+      <c r="Q121" s="1"/>
+      <c r="R121" s="32">
+        <v>1196095.82</v>
+      </c>
+      <c r="S121" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="T121" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20">
       <c r="A122" s="26"/>
       <c r="B122" s="26"/>
       <c r="C122" s="26"/>
@@ -9693,7 +10913,7 @@
       <c r="K122" s="26"/>
       <c r="L122" s="26"/>
       <c r="M122" s="26"/>
-      <c r="N122" s="26">
+      <c r="N122" s="29">
         <v>1196095.83</v>
       </c>
       <c r="O122" s="26" t="s">
@@ -9702,8 +10922,18 @@
       <c r="P122" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="123" spans="1:16">
+      <c r="Q122" s="1"/>
+      <c r="R122" s="32">
+        <v>1196095.83</v>
+      </c>
+      <c r="S122" s="26" t="s">
+        <v>507</v>
+      </c>
+      <c r="T122" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20">
       <c r="A123" s="26"/>
       <c r="B123" s="26"/>
       <c r="C123" s="26"/>
@@ -9717,7 +10947,7 @@
       <c r="K123" s="26"/>
       <c r="L123" s="26"/>
       <c r="M123" s="26"/>
-      <c r="N123" s="26">
+      <c r="N123" s="29">
         <v>1196095.8400000001</v>
       </c>
       <c r="O123" s="26" t="s">
@@ -9726,8 +10956,18 @@
       <c r="P123" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="124" spans="1:16">
+      <c r="Q123" s="1"/>
+      <c r="R123" s="32">
+        <v>1196095.8400000001</v>
+      </c>
+      <c r="S123" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="T123" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20">
       <c r="A124" s="26"/>
       <c r="B124" s="26"/>
       <c r="C124" s="26"/>
@@ -9741,7 +10981,7 @@
       <c r="K124" s="26"/>
       <c r="L124" s="26"/>
       <c r="M124" s="26"/>
-      <c r="N124" s="26">
+      <c r="N124" s="29">
         <v>1196095.8500000001</v>
       </c>
       <c r="O124" s="26" t="s">
@@ -9750,8 +10990,17 @@
       <c r="P124" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="125" spans="1:16">
+      <c r="R124" s="32">
+        <v>1196095.8500000001</v>
+      </c>
+      <c r="S124" s="26" t="s">
+        <v>538</v>
+      </c>
+      <c r="T124" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20">
       <c r="A125" s="26"/>
       <c r="B125" s="26"/>
       <c r="C125" s="26"/>
@@ -9765,7 +11014,7 @@
       <c r="K125" s="26"/>
       <c r="L125" s="26"/>
       <c r="M125" s="26"/>
-      <c r="N125" s="26">
+      <c r="N125" s="29">
         <v>1196095.8600000001</v>
       </c>
       <c r="O125" s="26" t="s">
@@ -9774,8 +11023,18 @@
       <c r="P125" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="126" spans="1:16">
+      <c r="Q125" s="1"/>
+      <c r="R125" s="32">
+        <v>1196095.8600000001</v>
+      </c>
+      <c r="S125" s="26" t="s">
+        <v>518</v>
+      </c>
+      <c r="T125" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20">
       <c r="A126" s="26"/>
       <c r="B126" s="26"/>
       <c r="C126" s="26"/>
@@ -9789,7 +11048,7 @@
       <c r="K126" s="26"/>
       <c r="L126" s="26"/>
       <c r="M126" s="26"/>
-      <c r="N126" s="26">
+      <c r="N126" s="29">
         <v>1196095.8700000001</v>
       </c>
       <c r="O126" s="26" t="s">
@@ -9798,8 +11057,18 @@
       <c r="P126" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="127" spans="1:16">
+      <c r="Q126" s="1"/>
+      <c r="R126" s="32">
+        <v>1196095.8700000001</v>
+      </c>
+      <c r="S126" s="26" t="s">
+        <v>519</v>
+      </c>
+      <c r="T126" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20">
       <c r="A127" s="26"/>
       <c r="B127" s="26"/>
       <c r="C127" s="26"/>
@@ -9813,7 +11082,7 @@
       <c r="K127" s="26"/>
       <c r="L127" s="26"/>
       <c r="M127" s="26"/>
-      <c r="N127" s="26">
+      <c r="N127" s="29">
         <v>1196095.8799999999</v>
       </c>
       <c r="O127" s="26" t="s">
@@ -9822,8 +11091,18 @@
       <c r="P127" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="128" spans="1:16">
+      <c r="Q127" s="1"/>
+      <c r="R127" s="32">
+        <v>1196095.8799999999</v>
+      </c>
+      <c r="S127" s="26" t="s">
+        <v>520</v>
+      </c>
+      <c r="T127" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20">
       <c r="A128" s="26"/>
       <c r="B128" s="26"/>
       <c r="C128" s="26"/>
@@ -9837,7 +11116,7 @@
       <c r="K128" s="26"/>
       <c r="L128" s="26"/>
       <c r="M128" s="26"/>
-      <c r="N128" s="26">
+      <c r="N128" s="29">
         <v>1196095.8899999999</v>
       </c>
       <c r="O128" s="26" t="s">
@@ -9846,8 +11125,18 @@
       <c r="P128" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="129" spans="1:16">
+      <c r="Q128" s="1"/>
+      <c r="R128" s="32">
+        <v>1196095.8899999999</v>
+      </c>
+      <c r="S128" s="26" t="s">
+        <v>521</v>
+      </c>
+      <c r="T128" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20">
       <c r="A129" s="26"/>
       <c r="B129" s="26"/>
       <c r="C129" s="26"/>
@@ -9861,7 +11150,7 @@
       <c r="K129" s="26"/>
       <c r="L129" s="26"/>
       <c r="M129" s="26"/>
-      <c r="N129" s="26">
+      <c r="N129" s="29">
         <v>1196095.8999999999</v>
       </c>
       <c r="O129" s="26" t="s">
@@ -9870,8 +11159,18 @@
       <c r="P129" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="130" spans="1:16">
+      <c r="Q129" s="1"/>
+      <c r="R129" s="32">
+        <v>1196095.8999999999</v>
+      </c>
+      <c r="S129" s="26" t="s">
+        <v>524</v>
+      </c>
+      <c r="T129" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20">
       <c r="A130" s="26"/>
       <c r="B130" s="26"/>
       <c r="C130" s="26"/>
@@ -9885,7 +11184,7 @@
       <c r="K130" s="26"/>
       <c r="L130" s="26"/>
       <c r="M130" s="26"/>
-      <c r="N130" s="26">
+      <c r="N130" s="29">
         <v>1196095.9099999999</v>
       </c>
       <c r="O130" s="26" t="s">
@@ -9894,8 +11193,17 @@
       <c r="P130" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="131" spans="1:16">
+      <c r="R130" s="32">
+        <v>1196095.9099999999</v>
+      </c>
+      <c r="S130" s="26" t="s">
+        <v>525</v>
+      </c>
+      <c r="T130" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20">
       <c r="A131" s="26"/>
       <c r="B131" s="26"/>
       <c r="C131" s="26"/>
@@ -9909,7 +11217,7 @@
       <c r="K131" s="26"/>
       <c r="L131" s="26"/>
       <c r="M131" s="26"/>
-      <c r="N131" s="26">
+      <c r="N131" s="29">
         <v>1196095.92</v>
       </c>
       <c r="O131" s="26" t="s">
@@ -9918,8 +11226,17 @@
       <c r="P131" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="132" spans="1:16">
+      <c r="R131" s="32">
+        <v>1196095.92</v>
+      </c>
+      <c r="S131" s="26" t="s">
+        <v>528</v>
+      </c>
+      <c r="T131" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20">
       <c r="A132" s="26"/>
       <c r="B132" s="26"/>
       <c r="C132" s="26"/>
@@ -9933,7 +11250,7 @@
       <c r="K132" s="26"/>
       <c r="L132" s="26"/>
       <c r="M132" s="26"/>
-      <c r="N132" s="26">
+      <c r="N132" s="29">
         <v>1196095.93</v>
       </c>
       <c r="O132" s="26" t="s">
@@ -9942,8 +11259,17 @@
       <c r="P132" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="133" spans="1:16">
+      <c r="R132" s="32">
+        <v>1196095.93</v>
+      </c>
+      <c r="S132" s="26" t="s">
+        <v>531</v>
+      </c>
+      <c r="T132" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20">
       <c r="A133" s="26"/>
       <c r="B133" s="26"/>
       <c r="C133" s="26"/>
@@ -9966,8 +11292,18 @@
       <c r="P133" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="134" spans="1:16">
+      <c r="Q133" s="1"/>
+      <c r="R133" s="32">
+        <v>1196095.94</v>
+      </c>
+      <c r="S133" t="s">
+        <v>379</v>
+      </c>
+      <c r="T133" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20">
       <c r="A134" s="26"/>
       <c r="B134" s="26"/>
       <c r="C134" s="26"/>
@@ -9981,7 +11317,7 @@
       <c r="K134" s="26"/>
       <c r="L134" s="26"/>
       <c r="M134" s="26"/>
-      <c r="N134">
+      <c r="N134" s="29">
         <v>1196095.95</v>
       </c>
       <c r="O134" t="s">
@@ -9990,8 +11326,18 @@
       <c r="P134" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="135" spans="1:16">
+      <c r="Q134" s="1"/>
+      <c r="R134" s="32">
+        <v>1196095.95</v>
+      </c>
+      <c r="S134" t="s">
+        <v>381</v>
+      </c>
+      <c r="T134" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20">
       <c r="A135" s="26"/>
       <c r="B135" s="26"/>
       <c r="C135" s="26"/>
@@ -10014,8 +11360,18 @@
       <c r="P135" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="136" spans="1:16">
+      <c r="Q135" s="1"/>
+      <c r="R135" s="32">
+        <v>1196095.96</v>
+      </c>
+      <c r="S135" t="s">
+        <v>384</v>
+      </c>
+      <c r="T135" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20">
       <c r="A136" s="26"/>
       <c r="B136" s="26"/>
       <c r="C136" s="26"/>
@@ -10038,8 +11394,18 @@
       <c r="P136" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="137" spans="1:16">
+      <c r="Q136" s="1"/>
+      <c r="R136" s="32">
+        <v>1196095.97</v>
+      </c>
+      <c r="S136" t="s">
+        <v>385</v>
+      </c>
+      <c r="T136" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20">
       <c r="A137" s="26"/>
       <c r="B137" s="26"/>
       <c r="C137" s="26"/>
@@ -10062,8 +11428,18 @@
       <c r="P137" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="1:16">
+      <c r="Q137" s="1"/>
+      <c r="R137" s="32">
+        <v>1196095.98</v>
+      </c>
+      <c r="S137" t="s">
+        <v>386</v>
+      </c>
+      <c r="T137" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20">
       <c r="A138" s="26"/>
       <c r="B138" s="26"/>
       <c r="C138" s="26"/>
@@ -10086,8 +11462,18 @@
       <c r="P138" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="139" spans="1:16">
+      <c r="Q138" s="1"/>
+      <c r="R138" s="32">
+        <v>1196095.99</v>
+      </c>
+      <c r="S138" t="s">
+        <v>387</v>
+      </c>
+      <c r="T138" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20">
       <c r="A139" s="26"/>
       <c r="B139" s="26"/>
       <c r="C139" s="26"/>
@@ -10110,8 +11496,18 @@
       <c r="P139" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="140" spans="1:16">
+      <c r="Q139" s="1"/>
+      <c r="R139" s="32">
+        <v>6666666.1644329997</v>
+      </c>
+      <c r="S139" t="s">
+        <v>492</v>
+      </c>
+      <c r="T139" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20">
       <c r="A140" s="26"/>
       <c r="B140" s="26"/>
       <c r="C140" s="26"/>
@@ -10134,8 +11530,18 @@
       <c r="P140" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="141" spans="1:16">
+      <c r="Q140" s="1"/>
+      <c r="R140" s="32">
+        <v>6666666.1644339999</v>
+      </c>
+      <c r="S140" t="s">
+        <v>495</v>
+      </c>
+      <c r="T140" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20">
       <c r="A141" s="26"/>
       <c r="B141" s="26"/>
       <c r="C141" s="26"/>
@@ -10158,8 +11564,18 @@
       <c r="P141" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="142" spans="1:16">
+      <c r="Q141" s="1"/>
+      <c r="R141" s="32">
+        <v>6666666.1644350002</v>
+      </c>
+      <c r="S141" t="s">
+        <v>496</v>
+      </c>
+      <c r="T141" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20">
       <c r="A142" s="26"/>
       <c r="B142" s="26"/>
       <c r="C142" s="26"/>
@@ -10182,8 +11598,18 @@
       <c r="P142" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="143" spans="1:16">
+      <c r="Q142" s="1"/>
+      <c r="R142" s="32">
+        <v>6666666.1644360004</v>
+      </c>
+      <c r="S142" t="s">
+        <v>498</v>
+      </c>
+      <c r="T142" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20">
       <c r="A143" s="26"/>
       <c r="B143" s="26"/>
       <c r="C143" s="26"/>
@@ -10206,8 +11632,18 @@
       <c r="P143" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="144" spans="1:16">
+      <c r="Q143" s="1"/>
+      <c r="R143" s="32">
+        <v>6666666.1644369997</v>
+      </c>
+      <c r="S143" t="s">
+        <v>499</v>
+      </c>
+      <c r="T143" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20">
       <c r="A144" s="26"/>
       <c r="B144" s="26"/>
       <c r="C144" s="26"/>
@@ -10230,8 +11666,18 @@
       <c r="P144" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="145" spans="1:16">
+      <c r="Q144" s="1"/>
+      <c r="R144" s="32">
+        <v>6666666.1644379999</v>
+      </c>
+      <c r="S144" s="26" t="s">
+        <v>508</v>
+      </c>
+      <c r="T144" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20">
       <c r="A145" s="26"/>
       <c r="B145" s="26"/>
       <c r="C145" s="26"/>
@@ -10254,8 +11700,18 @@
       <c r="P145" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="146" spans="1:16">
+      <c r="Q145" s="1"/>
+      <c r="R145" s="32">
+        <v>6666666.1644390002</v>
+      </c>
+      <c r="S145" s="26" t="s">
+        <v>511</v>
+      </c>
+      <c r="T145" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20">
       <c r="A146" s="26"/>
       <c r="B146" s="26"/>
       <c r="C146" s="26"/>
@@ -10278,8 +11734,18 @@
       <c r="P146" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="147" spans="1:16">
+      <c r="Q146" s="1"/>
+      <c r="R146" s="32">
+        <v>6666666.1644400004</v>
+      </c>
+      <c r="S146" s="26" t="s">
+        <v>512</v>
+      </c>
+      <c r="T146" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="147" spans="1:20">
       <c r="A147" s="26"/>
       <c r="B147" s="26"/>
       <c r="C147" s="26"/>
@@ -10302,8 +11768,18 @@
       <c r="P147" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="148" spans="1:16">
+      <c r="Q147" s="1"/>
+      <c r="R147" s="32">
+        <v>6666666.1644409997</v>
+      </c>
+      <c r="S147" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="T147" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="148" spans="1:20">
       <c r="A148" s="26"/>
       <c r="B148" s="26"/>
       <c r="C148" s="26"/>
@@ -10326,8 +11802,18 @@
       <c r="P148" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="149" spans="1:16">
+      <c r="Q148" s="1"/>
+      <c r="R148" s="32">
+        <v>6666666.1644430002</v>
+      </c>
+      <c r="S148" t="s">
+        <v>469</v>
+      </c>
+      <c r="T148" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="149" spans="1:20">
       <c r="A149" s="26"/>
       <c r="B149" s="26"/>
       <c r="C149" s="26"/>
@@ -10350,8 +11836,17 @@
       <c r="P149" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="150" spans="1:16">
+      <c r="R149" s="32">
+        <v>6666666.1644449998</v>
+      </c>
+      <c r="S149" s="26" t="s">
+        <v>534</v>
+      </c>
+      <c r="T149" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="150" spans="1:20">
       <c r="A150" s="26"/>
       <c r="B150" s="26"/>
       <c r="C150" s="26"/>
@@ -10374,8 +11869,17 @@
       <c r="P150" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="151" spans="1:16">
+      <c r="R150" s="32">
+        <v>6666666.164446</v>
+      </c>
+      <c r="S150" s="26" t="s">
+        <v>536</v>
+      </c>
+      <c r="T150" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="151" spans="1:20">
       <c r="A151" s="26"/>
       <c r="B151" s="26"/>
       <c r="C151" s="26"/>
@@ -10398,8 +11902,18 @@
       <c r="P151" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="152" spans="1:16">
+      <c r="Q151" s="1"/>
+      <c r="R151" s="32">
+        <v>6666666.1646299995</v>
+      </c>
+      <c r="S151" t="s">
+        <v>388</v>
+      </c>
+      <c r="T151" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="152" spans="1:20">
       <c r="A152" s="26"/>
       <c r="B152" s="26"/>
       <c r="C152" s="26"/>
@@ -10422,8 +11936,18 @@
       <c r="P152" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="153" spans="1:16">
+      <c r="Q152" s="1"/>
+      <c r="R152" s="32">
+        <v>6666666.1646389998</v>
+      </c>
+      <c r="S152" t="s">
+        <v>411</v>
+      </c>
+      <c r="T152" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="153" spans="1:20">
       <c r="A153" s="26"/>
       <c r="B153" s="26"/>
       <c r="C153" s="26"/>
@@ -10446,8 +11970,18 @@
       <c r="P153" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="154" spans="1:16">
+      <c r="Q153" s="1"/>
+      <c r="R153" s="32">
+        <v>6666666.1646400001</v>
+      </c>
+      <c r="S153" t="s">
+        <v>414</v>
+      </c>
+      <c r="T153" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="154" spans="1:20">
       <c r="A154" s="26"/>
       <c r="B154" s="26"/>
       <c r="C154" s="26"/>
@@ -10470,8 +12004,18 @@
       <c r="P154" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="155" spans="1:16">
+      <c r="Q154" s="1"/>
+      <c r="R154" s="32">
+        <v>6666666.1646410003</v>
+      </c>
+      <c r="S154" t="s">
+        <v>415</v>
+      </c>
+      <c r="T154" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="155" spans="1:20">
       <c r="A155" s="26"/>
       <c r="B155" s="26"/>
       <c r="C155" s="26"/>
@@ -10494,8 +12038,18 @@
       <c r="P155" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="156" spans="1:16">
+      <c r="Q155" s="1"/>
+      <c r="R155" s="32">
+        <v>6666666.1646419996</v>
+      </c>
+      <c r="S155" t="s">
+        <v>417</v>
+      </c>
+      <c r="T155" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="156" spans="1:20">
       <c r="A156" s="26"/>
       <c r="B156" s="26"/>
       <c r="C156" s="26"/>
@@ -10518,8 +12072,18 @@
       <c r="P156" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="157" spans="1:16">
+      <c r="Q156" s="1"/>
+      <c r="R156" s="32">
+        <v>6666666.1646429999</v>
+      </c>
+      <c r="S156" t="s">
+        <v>418</v>
+      </c>
+      <c r="T156" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="157" spans="1:20">
       <c r="A157" s="26"/>
       <c r="B157" s="26"/>
       <c r="C157" s="26"/>
@@ -10542,8 +12106,18 @@
       <c r="P157" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="158" spans="1:16">
+      <c r="Q157" s="1"/>
+      <c r="R157" s="32">
+        <v>6666666.1646459997</v>
+      </c>
+      <c r="S157" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="T157" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="158" spans="1:20">
       <c r="A158" s="26"/>
       <c r="B158" s="26"/>
       <c r="C158" s="26"/>
@@ -10566,8 +12140,18 @@
       <c r="P158" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="159" spans="1:16">
+      <c r="Q158" s="1"/>
+      <c r="R158" s="32">
+        <v>6666666.1646469999</v>
+      </c>
+      <c r="S158" s="26" t="s">
+        <v>430</v>
+      </c>
+      <c r="T158" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="159" spans="1:20">
       <c r="A159" s="26"/>
       <c r="B159" s="26"/>
       <c r="C159" s="26"/>
@@ -10590,8 +12174,18 @@
       <c r="P159" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="160" spans="1:16">
+      <c r="Q159" s="1"/>
+      <c r="R159" s="32">
+        <v>6666666.1646480002</v>
+      </c>
+      <c r="S159" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="T159" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="160" spans="1:20">
       <c r="A160" s="26"/>
       <c r="B160" s="26"/>
       <c r="C160" s="26"/>
@@ -10614,8 +12208,18 @@
       <c r="P160" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="161" spans="1:16">
+      <c r="Q160" s="1"/>
+      <c r="R160" s="32">
+        <v>6666666.1646499997</v>
+      </c>
+      <c r="S160" s="26" t="s">
+        <v>436</v>
+      </c>
+      <c r="T160" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="161" spans="1:20">
       <c r="A161" s="26"/>
       <c r="B161" s="26"/>
       <c r="C161" s="26"/>
@@ -10638,8 +12242,17 @@
       <c r="P161" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="162" spans="1:16">
+      <c r="R161" s="32">
+        <v>6666666.1646509999</v>
+      </c>
+      <c r="S161" s="26" t="s">
+        <v>453</v>
+      </c>
+      <c r="T161" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="162" spans="1:20">
       <c r="A162" s="26"/>
       <c r="B162" s="26"/>
       <c r="C162" s="26"/>
@@ -10662,6 +12275,15 @@
       <c r="P162" t="s">
         <v>344</v>
       </c>
+      <c r="R162" s="32">
+        <v>6666666.1646560002</v>
+      </c>
+      <c r="S162" s="26" t="s">
+        <v>455</v>
+      </c>
+      <c r="T162" t="s">
+        <v>344</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="B1:E162">

</xml_diff>